<commit_message>
Fixes to OBJECTIVE + LIGHTSOURCE + DETECTOR
</commit_message>
<xml_diff>
--- a/Model/in progress/v02-10/Components/Detector/NBO_MicroscopyMetadataSpecifications_DETECTOR_v02-10.xlsx
+++ b/Model/in progress/v02-10/Components/Detector/NBO_MicroscopyMetadataSpecifications_DETECTOR_v02-10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strambc/Documents/GitHub/NBOMicroscopyMetadataSpecs/Model/in progress/v02-10/Components/Detector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66BB9FF-D242-9749-B6ED-7FFD5BAC95CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338DBE95-02A7-AD4F-8534-B063F79238A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="900" windowWidth="26200" windowHeight="16320" activeTab="1" xr2:uid="{FF8EC58E-AC57-9D4D-AF0B-ECFDD46E717E}"/>
   </bookViews>
@@ -101,6 +101,7 @@
   <authors>
     <author/>
     <author>Strambio, Caterina</author>
+    <author>tc={3A71890E-D6C2-8C47-81E7-7957FF532473}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{1ED8C378-A4D3-6944-AE89-5365E66833F1}">
@@ -140,12 +141,22 @@
         </r>
       </text>
     </comment>
+    <comment ref="W1" authorId="2" shapeId="0" xr:uid="{3A71890E-D6C2-8C47-81E7-7957FF532473}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Use this column to provide feedback.
+Enter your name, lastname and email in the column header.
+Enter your comments/suggestions in the cell that corresponds to the row of the element/field you want to change.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="296">
   <si>
     <t>Tier</t>
   </si>
@@ -1045,7 +1056,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1286,6 +1297,12 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3218,6 +3235,16 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="W1" dT="2021-10-06T22:44:42.32" personId="{F8F8F373-FD67-9244-8810-9C85374FB326}" id="{3A71890E-D6C2-8C47-81E7-7957FF532473}">
+    <text>Use this column to provide feedback.
+Enter your name, lastname and email in the column header.
+Enter your comments/suggestions in the cell that corresponds to the row of the element/field you want to change.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93938140-A339-004E-8C0E-E2A9D19EA897}">
   <sheetPr>
@@ -3227,7 +3254,7 @@
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A79" sqref="A79:XFD79"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16738,11 +16765,11 @@
   <sheetPr>
     <tabColor rgb="FFBFBFBF"/>
   </sheetPr>
-  <dimension ref="A1:U855"/>
+  <dimension ref="A1:W855"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16760,7 +16787,9 @@
     <col min="16" max="16" width="12.33203125" style="253" customWidth="1"/>
     <col min="17" max="18" width="3.6640625" style="16" customWidth="1"/>
     <col min="19" max="21" width="12.33203125" style="16" customWidth="1"/>
-    <col min="22" max="24" width="10.83203125" style="16" customWidth="1"/>
+    <col min="22" max="22" width="10.83203125" style="16" customWidth="1"/>
+    <col min="23" max="23" width="24.1640625" style="263" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="16" customWidth="1"/>
     <col min="25" max="25" width="3.33203125" style="16" customWidth="1"/>
     <col min="26" max="28" width="10.83203125" style="16" customWidth="1"/>
     <col min="29" max="33" width="10.5" style="16" customWidth="1"/>
@@ -16768,7 +16797,7 @@
     <col min="47" max="16384" width="11.1640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="181" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="181" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16810,8 +16839,11 @@
       <c r="U1" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="W1" s="262" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="187"/>
       <c r="B2" s="187"/>
       <c r="C2" s="12"/>
@@ -16834,7 +16866,7 @@
       <c r="T2" s="14"/>
       <c r="U2" s="14"/>
     </row>
-    <row r="3" spans="1:21" s="29" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" s="29" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="182">
         <v>1</v>
       </c>
@@ -16870,8 +16902,9 @@
       <c r="U3" s="43" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="263"/>
+    </row>
+    <row r="4" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="187"/>
       <c r="B4" s="187"/>
       <c r="C4" s="12"/>
@@ -16894,7 +16927,7 @@
       <c r="T4" s="44"/>
       <c r="U4" s="43"/>
     </row>
-    <row r="5" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="182">
         <v>1</v>
       </c>
@@ -16933,7 +16966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="187"/>
       <c r="B6" s="187"/>
       <c r="C6" s="12"/>
@@ -16956,7 +16989,7 @@
       <c r="T6" s="44"/>
       <c r="U6" s="43"/>
     </row>
-    <row r="7" spans="1:21" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="201">
         <v>1</v>
       </c>
@@ -16991,7 +17024,7 @@
       <c r="T7" s="44"/>
       <c r="U7" s="43"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="187"/>
       <c r="B8" s="187"/>
       <c r="C8" s="12"/>
@@ -17014,7 +17047,7 @@
       <c r="T8" s="44"/>
       <c r="U8" s="43"/>
     </row>
-    <row r="9" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="182">
         <v>1</v>
       </c>
@@ -17050,8 +17083,11 @@
       <c r="U9" s="43" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W9" s="263" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="187"/>
       <c r="B10" s="187"/>
       <c r="C10" s="12"/>
@@ -17074,7 +17110,7 @@
       <c r="T10" s="44"/>
       <c r="U10" s="43"/>
     </row>
-    <row r="11" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="182">
         <v>1</v>
       </c>
@@ -17115,7 +17151,7 @@
       </c>
       <c r="U11" s="43"/>
     </row>
-    <row r="12" spans="1:21" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="182"/>
       <c r="B12" s="183"/>
       <c r="C12" s="12"/>
@@ -17142,7 +17178,7 @@
       <c r="T12" s="86"/>
       <c r="U12" s="85"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="182">
         <v>1</v>
       </c>
@@ -17181,7 +17217,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="182">
         <v>1</v>
       </c>
@@ -17220,7 +17256,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="182">
         <v>1</v>
       </c>
@@ -17259,7 +17295,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="182">
         <v>1</v>
       </c>

</xml_diff>